<commit_message>
20250917 Graceful Data loader
</commit_message>
<xml_diff>
--- a/GUI + Reviews/debug_output.xlsx
+++ b/GUI + Reviews/debug_output.xlsx
@@ -804,7 +804,7 @@
         <v>64</v>
       </c>
       <c r="J2">
-        <v>25.76</v>
+        <v>25.64</v>
       </c>
       <c r="K2">
         <v>25.87</v>
@@ -851,7 +851,7 @@
         <v>65</v>
       </c>
       <c r="J3">
-        <v>1345.2</v>
+        <v>1321</v>
       </c>
       <c r="K3">
         <v>1474.4</v>
@@ -898,7 +898,7 @@
         <v>66</v>
       </c>
       <c r="J4">
-        <v>6.64</v>
+        <v>6.54</v>
       </c>
       <c r="K4">
         <v>6.856</v>
@@ -945,7 +945,7 @@
         <v>67</v>
       </c>
       <c r="J5">
-        <v>34.32</v>
+        <v>33.67</v>
       </c>
       <c r="K5">
         <v>35.05</v>
@@ -992,7 +992,7 @@
         <v>68</v>
       </c>
       <c r="J6">
-        <v>61.2</v>
+        <v>60.86</v>
       </c>
       <c r="K6">
         <v>60.92</v>
@@ -1039,7 +1039,7 @@
         <v>116</v>
       </c>
       <c r="J7">
-        <v>29.59</v>
+        <v>29.4</v>
       </c>
       <c r="K7">
         <v>29.16</v>
@@ -1086,7 +1086,7 @@
         <v>70</v>
       </c>
       <c r="J8">
-        <v>424.5</v>
+        <v>455.9</v>
       </c>
       <c r="K8">
         <v>409.7</v>
@@ -1133,13 +1133,13 @@
         <v>71</v>
       </c>
       <c r="J9">
-        <v>689.8</v>
+        <v>732.9</v>
       </c>
       <c r="K9">
         <v>646.2</v>
       </c>
       <c r="L9">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M9" t="s">
         <v>113</v>
@@ -1180,7 +1180,7 @@
         <v>72</v>
       </c>
       <c r="J10">
-        <v>58.56</v>
+        <v>56.9</v>
       </c>
       <c r="K10">
         <v>63.26</v>
@@ -1227,7 +1227,7 @@
         <v>73</v>
       </c>
       <c r="J11">
-        <v>111.85</v>
+        <v>116.6</v>
       </c>
       <c r="K11">
         <v>119</v>
@@ -1274,7 +1274,7 @@
         <v>74</v>
       </c>
       <c r="J12">
-        <v>15.23</v>
+        <v>15.04</v>
       </c>
       <c r="K12">
         <v>17.53</v>
@@ -1321,7 +1321,7 @@
         <v>75</v>
       </c>
       <c r="J13">
-        <v>80.48</v>
+        <v>78.22</v>
       </c>
       <c r="K13">
         <v>84.94</v>
@@ -1368,7 +1368,7 @@
         <v>76</v>
       </c>
       <c r="J14">
-        <v>83.95</v>
+        <v>83.5</v>
       </c>
       <c r="K14">
         <v>87.25</v>
@@ -1415,7 +1415,7 @@
         <v>77</v>
       </c>
       <c r="J15">
-        <v>66</v>
+        <v>65.52</v>
       </c>
       <c r="K15">
         <v>70.86</v>
@@ -1462,7 +1462,7 @@
         <v>78</v>
       </c>
       <c r="J16">
-        <v>91.66</v>
+        <v>91.62</v>
       </c>
       <c r="K16">
         <v>95.7</v>
@@ -1509,7 +1509,7 @@
         <v>79</v>
       </c>
       <c r="J17">
-        <v>21.585</v>
+        <v>21.505</v>
       </c>
       <c r="K17">
         <v>21.32</v>
@@ -1556,7 +1556,7 @@
         <v>80</v>
       </c>
       <c r="J18">
-        <v>10.99</v>
+        <v>10.83</v>
       </c>
       <c r="K18">
         <v>13.13</v>
@@ -1603,7 +1603,7 @@
         <v>81</v>
       </c>
       <c r="J19">
-        <v>31.24</v>
+        <v>31.08</v>
       </c>
       <c r="K19">
         <v>26.54</v>
@@ -1697,7 +1697,7 @@
         <v>83</v>
       </c>
       <c r="J21">
-        <v>4.255</v>
+        <v>4.173</v>
       </c>
       <c r="K21">
         <v>4.062</v>
@@ -1744,7 +1744,7 @@
         <v>84</v>
       </c>
       <c r="J22">
-        <v>59.24</v>
+        <v>57.54</v>
       </c>
       <c r="K22">
         <v>61.26</v>
@@ -1791,7 +1791,7 @@
         <v>85</v>
       </c>
       <c r="J23">
-        <v>24.04</v>
+        <v>23.7</v>
       </c>
       <c r="K23">
         <v>24.07</v>
@@ -1838,7 +1838,7 @@
         <v>86</v>
       </c>
       <c r="J24">
-        <v>54.59</v>
+        <v>54.63</v>
       </c>
       <c r="K24">
         <v>53.61</v>
@@ -1885,13 +1885,13 @@
         <v>87</v>
       </c>
       <c r="J25">
-        <v>36.55</v>
+        <v>35.65</v>
       </c>
       <c r="K25">
         <v>41.69</v>
       </c>
       <c r="L25">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M25" t="s">
         <v>113</v>
@@ -1932,13 +1932,13 @@
         <v>88</v>
       </c>
       <c r="J26">
-        <v>39.78</v>
+        <v>39.44</v>
       </c>
       <c r="K26">
         <v>41.38</v>
       </c>
       <c r="L26">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M26" t="s">
         <v>113</v>
@@ -1979,7 +1979,7 @@
         <v>89</v>
       </c>
       <c r="J27">
-        <v>30.66</v>
+        <v>30.56</v>
       </c>
       <c r="K27">
         <v>31.225</v>
@@ -2026,7 +2026,7 @@
         <v>90</v>
       </c>
       <c r="J28">
-        <v>24.59</v>
+        <v>24.6</v>
       </c>
       <c r="K28">
         <v>24.81</v>
@@ -2073,7 +2073,7 @@
         <v>91</v>
       </c>
       <c r="J29">
-        <v>53.62</v>
+        <v>52.52</v>
       </c>
       <c r="K29">
         <v>53.98</v>
@@ -2120,7 +2120,7 @@
         <v>92</v>
       </c>
       <c r="J30">
-        <v>21.12</v>
+        <v>21.04</v>
       </c>
       <c r="K30">
         <v>22.48</v>
@@ -2167,7 +2167,7 @@
         <v>93</v>
       </c>
       <c r="J31">
-        <v>112.3</v>
+        <v>110.35</v>
       </c>
       <c r="K31">
         <v>115.3</v>
@@ -2214,7 +2214,7 @@
         <v>94</v>
       </c>
       <c r="J32">
-        <v>50</v>
+        <v>49.04</v>
       </c>
       <c r="K32">
         <v>54.24</v>
@@ -2261,13 +2261,13 @@
         <v>95</v>
       </c>
       <c r="J33">
-        <v>233.2</v>
+        <v>229.6</v>
       </c>
       <c r="K33">
         <v>229</v>
       </c>
       <c r="L33">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M33" t="s">
         <v>114</v>
@@ -2308,13 +2308,13 @@
         <v>96</v>
       </c>
       <c r="J34">
-        <v>62.9</v>
+        <v>62.7</v>
       </c>
       <c r="K34">
         <v>64.84999999999999</v>
       </c>
       <c r="L34">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M34" t="s">
         <v>114</v>
@@ -2355,7 +2355,7 @@
         <v>97</v>
       </c>
       <c r="J35">
-        <v>59.2</v>
+        <v>57.85</v>
       </c>
       <c r="K35">
         <v>62.5</v>
@@ -2402,7 +2402,7 @@
         <v>98</v>
       </c>
       <c r="J36">
-        <v>644.4</v>
+        <v>630.6</v>
       </c>
       <c r="K36">
         <v>565.6</v>
@@ -2449,7 +2449,7 @@
         <v>99</v>
       </c>
       <c r="J37">
-        <v>11.87</v>
+        <v>12.18</v>
       </c>
       <c r="K37">
         <v>13.48</v>
@@ -2496,7 +2496,7 @@
         <v>100</v>
       </c>
       <c r="J38">
-        <v>73.90000000000001</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="K38">
         <v>76.3</v>
@@ -2543,7 +2543,7 @@
         <v>101</v>
       </c>
       <c r="J39">
-        <v>165.3</v>
+        <v>162.2</v>
       </c>
       <c r="K39">
         <v>190.8</v>
@@ -2590,7 +2590,7 @@
         <v>102</v>
       </c>
       <c r="J40">
-        <v>95.25</v>
+        <v>95.34999999999999</v>
       </c>
       <c r="K40">
         <v>99.45</v>
@@ -2637,13 +2637,13 @@
         <v>103</v>
       </c>
       <c r="J41">
-        <v>76</v>
+        <v>74.3</v>
       </c>
       <c r="K41">
         <v>76.7</v>
       </c>
       <c r="L41">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M41" t="s">
         <v>114</v>
@@ -2684,7 +2684,7 @@
         <v>104</v>
       </c>
       <c r="J42">
-        <v>101.85</v>
+        <v>100.85</v>
       </c>
       <c r="K42">
         <v>104.9</v>
@@ -2731,7 +2731,7 @@
         <v>105</v>
       </c>
       <c r="J43">
-        <v>8350</v>
+        <v>8100</v>
       </c>
       <c r="K43">
         <v>8220</v>
@@ -2778,7 +2778,7 @@
         <v>106</v>
       </c>
       <c r="J44">
-        <v>65.55</v>
+        <v>64.45</v>
       </c>
       <c r="K44">
         <v>68.40000000000001</v>
@@ -2825,13 +2825,13 @@
         <v>107</v>
       </c>
       <c r="J45">
-        <v>66.7</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="K45">
         <v>70</v>
       </c>
       <c r="L45">
-        <v>1.1727</v>
+        <v>1.1852</v>
       </c>
       <c r="M45" t="s">
         <v>114</v>
@@ -2872,7 +2872,7 @@
         <v>108</v>
       </c>
       <c r="J46">
-        <v>252.8</v>
+        <v>249.6</v>
       </c>
       <c r="K46">
         <v>266.4</v>
@@ -2891,6 +2891,9 @@
       </c>
     </row>
     <row r="47" spans="1:15">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="B47" t="s">
         <v>60</v>
       </c>
@@ -2935,6 +2938,9 @@
       </c>
     </row>
     <row r="48" spans="1:15">
+      <c r="A48">
+        <v>47</v>
+      </c>
       <c r="B48" t="s">
         <v>61</v>
       </c>
@@ -2960,7 +2966,7 @@
         <v>110</v>
       </c>
       <c r="J48">
-        <v>72.12</v>
+        <v>71.72</v>
       </c>
       <c r="K48">
         <v>78.28</v>
@@ -2978,7 +2984,10 @@
         <v>0.7000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <v>48</v>
+      </c>
       <c r="B49" t="s">
         <v>62</v>
       </c>
@@ -3004,7 +3013,7 @@
         <v>111</v>
       </c>
       <c r="J49">
-        <v>207.4</v>
+        <v>203.9</v>
       </c>
       <c r="K49">
         <v>197.3</v>
@@ -3022,7 +3031,10 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <v>49</v>
+      </c>
       <c r="B50" t="s">
         <v>63</v>
       </c>
@@ -3048,7 +3060,7 @@
         <v>112</v>
       </c>
       <c r="J50">
-        <v>13.16</v>
+        <v>12.78</v>
       </c>
       <c r="K50">
         <v>13.88</v>
@@ -3066,7 +3078,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="1:15">
+      <c r="A51">
+        <v>50</v>
+      </c>
       <c r="B51" t="s">
         <v>43</v>
       </c>
@@ -3092,7 +3107,7 @@
         <v>92</v>
       </c>
       <c r="J51">
-        <v>21.12</v>
+        <v>21.04</v>
       </c>
       <c r="K51">
         <v>22.48</v>

</xml_diff>